<commit_message>
updated analysis on experiments
updated excel charts and documentation
</commit_message>
<xml_diff>
--- a/Analysis/2kr_analysis/boss_arrival_time_20-30/throughput/hard_game_mode/2kr_hard_minion_throughput.xlsx
+++ b/Analysis/2kr_analysis/boss_arrival_time_20-30/throughput/hard_game_mode/2kr_hard_minion_throughput.xlsx
@@ -302,11 +302,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
@@ -315,6 +310,11 @@
     </font>
     <font>
       <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -743,7 +743,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -767,7 +767,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -852,7 +852,7 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF9C0006"/>
+      <rgbColor rgb="FF7E0021"/>
       <rgbColor rgb="FF006100"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
@@ -873,7 +873,7 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF9C0006"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
@@ -887,13 +887,13 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFFD320"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF004586"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF579D1C"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -905,7 +905,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1978,11 +1978,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="71249655"/>
-        <c:axId val="94035262"/>
+        <c:axId val="5434470"/>
+        <c:axId val="448810"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71249655"/>
+        <c:axId val="5434470"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2038,12 +2038,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94035262"/>
+        <c:crossAx val="448810"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94035262"/>
+        <c:axId val="448810"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2108,7 +2108,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71249655"/>
+        <c:crossAx val="5434470"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2135,7 +2135,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2216,10 +2216,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$X$69:$X$228</c:f>
+              <c:f>Sheet1!$X$69:$X$100</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="160"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>0.09888</c:v>
                 </c:pt>
@@ -2314,390 +2314,6 @@
                   <c:v>0.06784</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.06768</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.09888</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.09856</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.08928</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.08272</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.06768</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.06768</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.06664</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.06544</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.09592</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.09552</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.07392</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.06832</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.06696</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.06672</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.0616</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.05984</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.1012</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.1012</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.09816</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0.09488</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0.06816</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>0.06816</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>0.06808</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0.06792</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0.10104</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0.10104</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0.0924</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0.0888</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>0.06816</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>0.06816</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0.06784</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>0.06768</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>0.09888</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0.09856</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>0.08928</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0.08272</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>0.06768</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>0.06768</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>0.06664</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>0.06544</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>0.09592</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>0.09552</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>0.07392</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>0.06832</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>0.06696</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>0.06672</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>0.0616</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>0.05984</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0.1012</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>0.1012</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>0.09816</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>0.09488</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>0.06816</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0.06816</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0.06808</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0.06792</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0.10104</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>0.10104</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>0.0924</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>0.0888</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0.06816</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0.06816</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>0.06784</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>0.06768</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>0.09888</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>0.09856</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>0.08928</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0.08272</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>0.06768</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>0.06768</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>0.06664</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>0.06544</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>0.09592</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>0.09552</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>0.07392</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>0.06832</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>0.06696</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>0.06672</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>0.0616</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>0.05984</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>0.1012</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>0.1012</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>0.09816</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>0.09488</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>0.06816</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>0.06816</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>0.06808</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>0.06792</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>0.10104</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>0.10104</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>0.0924</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>0.0888</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>0.06816</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>0.06816</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>0.06784</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>0.06768</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>0.09888</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>0.09856</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>0.08928</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>0.08272</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>0.06768</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>0.06768</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>0.06664</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>0.06544</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>0.09592</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>0.09552</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>0.07392</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>0.06832</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>0.06696</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>0.06672</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>0.0616</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>0.05984</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>0.1012</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>0.1012</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>0.09816</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>0.09488</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>0.06816</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>0.06816</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>0.06808</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>0.06792</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>0.10104</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>0.10104</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>0.0924</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>0.0888</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>0.06816</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>0.06816</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>0.06784</c:v>
-                </c:pt>
-                <c:pt idx="159">
                   <c:v>0.06768</c:v>
                 </c:pt>
               </c:numCache>
@@ -2705,10 +2321,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Y$69:$Y$228</c:f>
+              <c:f>Sheet1!$Y$69:$Y$100</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="160"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>-0.00248</c:v>
                 </c:pt>
@@ -2804,401 +2420,1025 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>-0.00488</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>-7.99999999999967E-005</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>-0.000560000000000005</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>-0.00367999999999999</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>-0.00711999999999999</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.000719999999999998</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.000719999999999998</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>-0.000640000000000002</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>-0.00023999999999999</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.00168</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.000879999999999992</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>-0.00152000000000001</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>-0.00192000000000001</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.00144000000000001</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.00168</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.00239999999999999</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>-0.000240000000000004</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>-0.00199999999999999</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>-0.00199999999999999</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>-0.00295999999999999</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>-0.00407999999999999</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0.00023999999999999</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>0.00023999999999999</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>0.000320000000000001</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>-0.000320000000000001</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>-0.00184000000000001</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>-0.00184000000000001</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>-0.00280000000000001</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>-0.0044</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>0.00023999999999999</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>0.00023999999999999</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>-0.00023999999999999</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>-7.99999999999967E-005</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>-0.00327999999999999</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>-0.00336</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>-0.01408</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>-0.01192</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>0.00192000000000001</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>0.00192000000000001</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>0.00136</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>-0.000640000000000002</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>-0.00512</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>-0.00552000000000001</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>-0.01952</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>-0.01752</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>0.000240000000000018</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>-0.000320000000000001</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>-0.01</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>-0.01224</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0.0016</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>0.0016</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>-0.000559999999999991</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>-0.00407999999999999</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>0.00343999999999998</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0.00343999999999998</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0.00352</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0.00367999999999999</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0.000959999999999989</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>0.000959999999999989</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>-0.0064</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>-0.0072</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0.00343999999999998</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0.00343999999999998</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>0.00376</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>0.00391999999999999</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>0.00472000000000002</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>0.00504</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>0.00952</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0.01088</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>-0.00128</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>-0.00128</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>-0.000640000000000002</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>0.000560000000000005</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>0.00568</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>0.00608</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>0.01168</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>0.01088</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>-0.00135999999999999</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>-0.00112</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>0.004</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>0.00576</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>0.00520000000000001</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>0.00520000000000001</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>0.00464000000000001</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>0.00392000000000001</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>-0.00136000000000001</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>-0.00136000000000001</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>-0.00128</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>-0.00112000000000001</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>0.00535999999999999</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>0.00535999999999999</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>0.0048</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>0.0072</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>-0.00136000000000001</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>-0.00136000000000001</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>-0.00104</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>-0.000880000000000006</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>0.00112000000000001</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>0.00104</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>0.00352000000000001</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>0.00448000000000001</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>0.00192000000000001</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>0.00192000000000001</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>0.00216</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>0.00176000000000001</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>-0.00272</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>-0.00232</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>0.00248</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>0.00527999999999999</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>0.00224000000000001</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>0.00208</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>0.0012</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>0.00296</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>0.000640000000000002</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>0.00272000000000001</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>0.00144</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>0.00144</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>0.00152000000000001</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>0.00168</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>0.00015999999999998</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>0.00015999999999998</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>0.0048</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>0.0064</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>0.00144</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>0.00144</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>0.00176000000000001</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>0.00192000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="86300396"/>
-        <c:axId val="99778909"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$X$69:$X$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>0.09888</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.09856</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.08928</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.08272</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.06768</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.06664</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.06544</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.09592</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.09552</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.07392</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.06832</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.06696</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.06672</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0616</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.05984</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.1012</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.1012</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.09816</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.09488</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.06816</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.06816</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.06808</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.06792</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.10104</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.10104</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.0924</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.0888</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.06816</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.06816</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.06784</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.06768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$Y$101:$Y$132</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>-7.99999999999967E-005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.000560000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.00367999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.00711999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.000719999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.000719999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.000640000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.00023999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.00168</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.000879999999999992</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.00152000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.00192000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.00144000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.00168</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.00239999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.000240000000000004</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-0.00199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-0.00199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-0.00295999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-0.00407999999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.00023999999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.00023999999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.000320000000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-0.000320000000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-0.00184000000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-0.00184000000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-0.00280000000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-0.0044</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.00023999999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.00023999999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-0.00023999999999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-7.99999999999967E-005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$X$69:$X$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>0.09888</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.09856</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.08928</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.08272</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.06768</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.06664</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.06544</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.09592</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.09552</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.07392</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.06832</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.06696</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.06672</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0616</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.05984</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.1012</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.1012</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.09816</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.09488</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.06816</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.06816</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.06808</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.06792</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.10104</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.10104</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.0924</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.0888</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.06816</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.06816</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.06784</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.06768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$Y$133:$Y$164</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>-0.00327999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.00336</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.01408</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.01192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.00192000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00192000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.00136</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.000640000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.00512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.00552000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.01952</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.01752</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.000240000000000018</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.000320000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.01</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.01224</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.0016</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.0016</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-0.000559999999999991</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-0.00407999999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.00343999999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.00343999999999998</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.00352</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.00367999999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.000959999999999989</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.000959999999999989</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-0.0064</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-0.0072</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.00343999999999998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.00343999999999998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.00376</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.00391999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="579d1c"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$X$69:$X$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>0.09888</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.09856</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.08928</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.08272</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.06768</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.06664</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.06544</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.09592</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.09552</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.07392</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.06832</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.06696</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.06672</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0616</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.05984</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.1012</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.1012</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.09816</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.09488</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.06816</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.06816</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.06808</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.06792</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.10104</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.10104</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.0924</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.0888</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.06816</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.06816</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.06784</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.06768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$Y$165:$Y$196</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>0.00472000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00504</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00952</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01088</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.00128</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.00128</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.000640000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.000560000000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.00568</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.00608</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.01168</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.01088</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.00135999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.00112</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.00576</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.00520000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.00520000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.00464000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.00392000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-0.00136000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-0.00136000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-0.00128</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-0.00112000000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.00535999999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.00535999999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.0048</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.0072</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-0.00136000000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-0.00136000000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-0.00104</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-0.000880000000000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="7e0021"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$X$69:$X$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>0.09888</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.09856</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.08928</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.08272</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.06768</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.06664</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.06544</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.09592</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.09552</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.07392</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.06832</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.06696</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.06672</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0616</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.05984</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.1012</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.1012</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.09816</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.09488</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.06816</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.06816</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.06808</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.06792</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.10104</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.10104</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.0924</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.0888</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.06816</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.06816</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.06784</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.06768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$Y$197:$Y$228</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>0.00112000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00104</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00352000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.00448000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.00192000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00192000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.00216</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.00176000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.00272</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.00232</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.00248</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.00527999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.00224000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.00208</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0012</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.00296</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.000640000000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.00272000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.00144</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.00144</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.00152000000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.00168</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.00015999999999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.00015999999999998</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.0048</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.0064</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.00144</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.00144</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.00176000000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.00192000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="23520051"/>
+        <c:axId val="96461201"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86300396"/>
+        <c:axId val="23520051"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3254,12 +3494,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99778909"/>
+        <c:crossAx val="96461201"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99778909"/>
+        <c:axId val="96461201"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3324,7 +3564,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86300396"/>
+        <c:crossAx val="23520051"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3362,9 +3602,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>524520</xdr:colOff>
+      <xdr:colOff>524160</xdr:colOff>
       <xdr:row>96</xdr:row>
-      <xdr:rowOff>77400</xdr:rowOff>
+      <xdr:rowOff>77040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3372,8 +3612,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11061360" y="11786400"/>
-        <a:ext cx="7594920" cy="4550040"/>
+        <a:off x="11066400" y="11786400"/>
+        <a:ext cx="7605720" cy="4549680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3392,9 +3632,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>493560</xdr:colOff>
+      <xdr:colOff>493200</xdr:colOff>
       <xdr:row>93</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3402,8 +3642,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="28607400" y="11750040"/>
-        <a:ext cx="7018560" cy="4133520"/>
+        <a:off x="28638000" y="11750040"/>
+        <a:ext cx="7028280" cy="4133160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3423,11 +3663,11 @@
   </sheetPr>
   <dimension ref="A1:BP228"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AR56" activeCellId="0" sqref="AR56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W61" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AC84" activeCellId="0" sqref="AC84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.57"/>

</xml_diff>